<commit_message>
made some last minute fixes after realizing some cells from the excel test file and junit tests did not match up. should be the last commit
</commit_message>
<xml_diff>
--- a/ClueFiles/ClueBoardTests.xlsx
+++ b/ClueFiles/ClueBoardTests.xlsx
@@ -506,8 +506,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1727,7 +1727,7 @@
       <c r="D17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F17" s="3" t="s">
@@ -1802,7 +1802,7 @@
       <c r="D18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="10" t="s">
         <v>11</v>
       </c>
       <c r="F18" s="3" t="s">

</xml_diff>